<commit_message>
extended training and friends
</commit_message>
<xml_diff>
--- a/outputs/missing_answer_entity_analysis/missing_answer_entity_sheet_concluded.xlsx
+++ b/outputs/missing_answer_entity_analysis/missing_answer_entity_sheet_concluded.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lasse\Documents\6sem\Project\dataset-generation\outputs\missing_answer_entity_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{58E6BCBA-8AC1-41CC-9935-9EC9619C83CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{667CAD02-383D-47B1-9BA5-01CAB6A3C6F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="5" r:id="rId1"/>
@@ -3152,7 +3152,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -3162,14 +3162,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -3750,8 +3746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5441E6B6-FD25-4356-9537-69CC0A1F316F}">
   <dimension ref="B6:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3762,244 +3758,175 @@
     <col min="7" max="7" width="10.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B25" s="15"/>
-      <c r="C25" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="15" t="s">
+      <c r="B25" s="11"/>
+      <c r="C25" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="E25" s="15" t="s">
+      <c r="E25" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="F25" s="15" t="s">
+      <c r="F25" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="G25" s="15" t="s">
+      <c r="G25" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H25" s="15" t="s">
+      <c r="H25" s="11" t="s">
         <v>592</v>
       </c>
-      <c r="I25" s="15" t="s">
+      <c r="I25" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="J25" s="15" t="s">
+      <c r="J25" s="11" t="s">
         <v>507</v>
       </c>
-      <c r="K25" s="15" t="s">
+      <c r="K25" s="11" t="s">
         <v>999</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="12" t="s">
         <v>996</v>
       </c>
-      <c r="C26" s="17">
+      <c r="C26" s="13">
         <v>11</v>
       </c>
-      <c r="D26" s="17">
+      <c r="D26" s="13">
         <v>1</v>
       </c>
-      <c r="E26" s="17">
+      <c r="E26" s="13">
         <v>5</v>
       </c>
-      <c r="F26" s="17">
+      <c r="F26" s="13">
         <v>1</v>
       </c>
-      <c r="G26" s="17">
+      <c r="G26" s="13">
         <v>1</v>
       </c>
-      <c r="H26" s="17">
+      <c r="H26" s="13">
         <v>0</v>
       </c>
-      <c r="I26" s="17">
+      <c r="I26" s="13">
         <v>0</v>
       </c>
-      <c r="J26" s="17">
+      <c r="J26" s="13">
         <v>0</v>
       </c>
-      <c r="K26" s="18">
+      <c r="K26" s="14">
         <f>SUM(C26:J26)</f>
         <v>19</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="12" t="s">
         <v>997</v>
       </c>
-      <c r="C27" s="17">
+      <c r="C27" s="13">
         <v>20</v>
       </c>
-      <c r="D27" s="17">
+      <c r="D27" s="13">
         <v>1</v>
       </c>
-      <c r="E27" s="17">
+      <c r="E27" s="13">
         <v>26</v>
       </c>
-      <c r="F27" s="17">
+      <c r="F27" s="13">
         <v>5</v>
       </c>
-      <c r="G27" s="17">
+      <c r="G27" s="13">
         <v>2</v>
       </c>
-      <c r="H27" s="17">
+      <c r="H27" s="13">
         <v>0</v>
       </c>
-      <c r="I27" s="17">
+      <c r="I27" s="13">
         <v>13</v>
       </c>
-      <c r="J27" s="17">
+      <c r="J27" s="13">
         <v>0</v>
       </c>
-      <c r="K27" s="18">
+      <c r="K27" s="14">
         <f t="shared" ref="K27:K29" si="0">SUM(C27:J27)</f>
         <v>67</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="12" t="s">
         <v>998</v>
       </c>
-      <c r="C28" s="17">
+      <c r="C28" s="13">
         <v>73</v>
       </c>
-      <c r="D28" s="17">
+      <c r="D28" s="13">
         <v>4</v>
       </c>
-      <c r="E28" s="17">
+      <c r="E28" s="13">
         <v>67</v>
       </c>
-      <c r="F28" s="17">
+      <c r="F28" s="13">
         <v>17</v>
       </c>
-      <c r="G28" s="17">
+      <c r="G28" s="13">
         <v>6</v>
       </c>
-      <c r="H28" s="17">
+      <c r="H28" s="13">
         <v>6</v>
       </c>
-      <c r="I28" s="17">
+      <c r="I28" s="13">
         <v>32</v>
       </c>
-      <c r="J28" s="17">
+      <c r="J28" s="13">
         <v>4</v>
       </c>
-      <c r="K28" s="18">
+      <c r="K28" s="14">
         <f t="shared" si="0"/>
         <v>209</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B29" s="16" t="s">
+      <c r="B29" s="12" t="s">
         <v>999</v>
       </c>
-      <c r="C29" s="18">
+      <c r="C29" s="14">
         <f>SUM(C26:C28)</f>
         <v>104</v>
       </c>
-      <c r="D29" s="18">
+      <c r="D29" s="14">
         <f t="shared" ref="D29:G29" si="1">SUM(D26:D28)</f>
         <v>6</v>
       </c>
-      <c r="E29" s="18">
+      <c r="E29" s="14">
         <f t="shared" si="1"/>
         <v>98</v>
       </c>
-      <c r="F29" s="18">
+      <c r="F29" s="14">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="G29" s="18">
+      <c r="G29" s="14">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="H29" s="18">
+      <c r="H29" s="14">
         <f t="shared" ref="H29" si="2">SUM(H26:H28)</f>
         <v>6</v>
       </c>
-      <c r="I29" s="18">
+      <c r="I29" s="14">
         <f t="shared" ref="I29" si="3">SUM(I26:I28)</f>
         <v>45</v>
       </c>
-      <c r="J29" s="18">
+      <c r="J29" s="14">
         <f t="shared" ref="J29" si="4">SUM(J26:J28)</f>
         <v>4</v>
       </c>
-      <c r="K29" s="18">
+      <c r="K29" s="14">
         <f t="shared" si="0"/>
         <v>295</v>
       </c>
@@ -4055,10 +3982,10 @@
       <c r="G1" s="1" t="s">
         <v>966</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>969</v>
       </c>
-      <c r="I1" s="13"/>
+      <c r="I1" s="9"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -4082,10 +4009,10 @@
       <c r="G2" t="s">
         <v>968</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="8" t="s">
         <v>970</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="10" t="s">
         <v>979</v>
       </c>
       <c r="K2" t="s">
@@ -4126,10 +4053,10 @@
       <c r="G3" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="8" t="s">
         <v>987</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="10" t="s">
         <v>979</v>
       </c>
       <c r="J3" t="s">
@@ -4178,10 +4105,10 @@
       <c r="G4" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="8" t="s">
         <v>971</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I4" s="10" t="s">
         <v>979</v>
       </c>
       <c r="J4" t="s">
@@ -4230,10 +4157,10 @@
       <c r="G5" t="s">
         <v>972</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="8" t="s">
         <v>973</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="10" t="s">
         <v>979</v>
       </c>
       <c r="J5" t="s">
@@ -4282,10 +4209,10 @@
       <c r="G6" t="s">
         <v>974</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="8" t="s">
         <v>975</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="I6" s="10" t="s">
         <v>979</v>
       </c>
       <c r="J6" t="s">
@@ -4329,13 +4256,13 @@
       <c r="G7" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="8" t="s">
         <v>976</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="I7" s="10" t="s">
         <v>979</v>
       </c>
-      <c r="J7" s="11" t="s">
+      <c r="J7" t="s">
         <v>995</v>
       </c>
       <c r="K7" s="4">
@@ -4376,13 +4303,12 @@
       <c r="G8" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="8" t="s">
         <v>977</v>
       </c>
-      <c r="I8" s="14" t="s">
+      <c r="I8" s="10" t="s">
         <v>979</v>
       </c>
-      <c r="J8" s="11"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -4406,13 +4332,12 @@
       <c r="G9" t="s">
         <v>978</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H9" s="8" t="s">
         <v>981</v>
       </c>
-      <c r="I9" s="14" t="s">
+      <c r="I9" s="10" t="s">
         <v>979</v>
       </c>
-      <c r="J9" s="11"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -4436,13 +4361,12 @@
       <c r="G10" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H10" s="8" t="s">
         <v>980</v>
       </c>
-      <c r="I10" s="14" t="s">
+      <c r="I10" s="10" t="s">
         <v>979</v>
       </c>
-      <c r="J10" s="11"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -4466,13 +4390,12 @@
       <c r="G11" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="H11" s="8" t="s">
         <v>982</v>
       </c>
-      <c r="I11" s="14" t="s">
+      <c r="I11" s="10" t="s">
         <v>979</v>
       </c>
-      <c r="J11" s="11"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -4496,13 +4419,12 @@
       <c r="G12" t="s">
         <v>983</v>
       </c>
-      <c r="H12" s="9" t="s">
+      <c r="H12" s="8" t="s">
         <v>984</v>
       </c>
-      <c r="I12" s="14" t="s">
+      <c r="I12" s="10" t="s">
         <v>979</v>
       </c>
-      <c r="J12" s="11"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -4526,13 +4448,12 @@
       <c r="G13" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="9" t="s">
+      <c r="H13" s="8" t="s">
         <v>985</v>
       </c>
-      <c r="I13" s="14" t="s">
+      <c r="I13" s="10" t="s">
         <v>979</v>
       </c>
-      <c r="J13" s="11"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -4556,13 +4477,12 @@
       <c r="G14" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="9" t="s">
+      <c r="H14" s="8" t="s">
         <v>986</v>
       </c>
-      <c r="I14" s="14" t="s">
+      <c r="I14" s="10" t="s">
         <v>979</v>
       </c>
-      <c r="J14" s="12"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -4586,13 +4506,12 @@
       <c r="G15" t="s">
         <v>15</v>
       </c>
-      <c r="H15" s="9" t="s">
+      <c r="H15" s="8" t="s">
         <v>988</v>
       </c>
-      <c r="I15" s="14" t="s">
+      <c r="I15" s="10" t="s">
         <v>979</v>
       </c>
-      <c r="J15" s="12"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
@@ -4616,15 +4535,14 @@
       <c r="G16" t="s">
         <v>15</v>
       </c>
-      <c r="H16" s="9" t="s">
+      <c r="H16" s="8" t="s">
         <v>989</v>
       </c>
-      <c r="I16" s="14" t="s">
+      <c r="I16" s="10" t="s">
         <v>979</v>
       </c>
-      <c r="J16" s="12"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>73</v>
       </c>
@@ -4646,15 +4564,14 @@
       <c r="G17" t="s">
         <v>990</v>
       </c>
-      <c r="H17" s="9" t="s">
+      <c r="H17" s="8" t="s">
         <v>991</v>
       </c>
-      <c r="I17" s="14" t="s">
+      <c r="I17" s="10" t="s">
         <v>979</v>
       </c>
-      <c r="J17" s="12"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>77</v>
       </c>
@@ -4676,15 +4593,14 @@
       <c r="G18" t="s">
         <v>15</v>
       </c>
-      <c r="H18" s="9" t="s">
+      <c r="H18" s="8" t="s">
         <v>992</v>
       </c>
-      <c r="I18" s="14" t="s">
+      <c r="I18" s="10" t="s">
         <v>979</v>
       </c>
-      <c r="J18" s="12"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>82</v>
       </c>
@@ -4706,15 +4622,14 @@
       <c r="G19" t="s">
         <v>15</v>
       </c>
-      <c r="H19" s="9" t="s">
+      <c r="H19" s="8" t="s">
         <v>993</v>
       </c>
-      <c r="I19" s="14" t="s">
+      <c r="I19" s="10" t="s">
         <v>979</v>
       </c>
-      <c r="J19" s="12"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>85</v>
       </c>
@@ -4736,15 +4651,14 @@
       <c r="G20" t="s">
         <v>15</v>
       </c>
-      <c r="H20" s="9" t="s">
+      <c r="H20" s="8" t="s">
         <v>994</v>
       </c>
-      <c r="I20" s="14" t="s">
+      <c r="I20" s="10" t="s">
         <v>979</v>
       </c>
-      <c r="J20" s="12"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B26" s="5"/>
     </row>
   </sheetData>

</xml_diff>